<commit_message>
Added initial Contract tree.
</commit_message>
<xml_diff>
--- a/spreadsheets/items.xlsx
+++ b/spreadsheets/items.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\production-line\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904F978B-0A55-4B0D-808E-BB835BDF4B60}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4C3450-E34D-491C-8A41-F1C800AF1940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37110" windowHeight="14625" xr2:uid="{90F13507-3F9A-4BE5-82EE-4FDD9857C5A2}"/>
   </bookViews>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642C1486-BA39-4873-8BE1-FD047E7D1A0C}">
   <dimension ref="A1:I81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,23 +1583,17 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A27, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>68</v>
-      </c>
-      <c r="F27" t="s">
-        <v>159</v>
+        <v>72</v>
       </c>
       <c r="G27">
         <v>1</v>
@@ -1607,17 +1601,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B28">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A28, ":"),D$2:D$125)))</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
+      <c r="D28" t="s">
+        <v>78</v>
+      </c>
       <c r="E28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1625,7 +1622,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B29">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A29, ":"),D$2:D$125)))</f>
@@ -1635,10 +1632,10 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1646,20 +1643,17 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B30">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A30, ":"),D$2:D$125)))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
-      <c r="D30" t="s">
-        <v>86</v>
-      </c>
       <c r="E30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1667,17 +1661,20 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B31">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A31, ":"),D$2:D$125)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1685,7 +1682,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A32, ":"),D$2:D$125)))</f>
@@ -1695,77 +1692,77 @@
         <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>26</v>
+      <c r="A33" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="B33">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A33, ":"),D$2:D$125)))</f>
         <v>1</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>88</v>
-      </c>
-      <c r="E33" t="s">
-        <v>71</v>
-      </c>
+      <c r="C33" s="6">
+        <v>0</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F33" s="6"/>
       <c r="G33">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="B34">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$125)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="F34" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>159</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>175</v>
+      <c r="A35" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B35">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A35, ":"),D$2:D$125)))</f>
-        <v>0</v>
-      </c>
-      <c r="C35" s="6">
-        <v>1</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>159</v>
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" t="s">
+        <v>73</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1773,20 +1770,20 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B36">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A36, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1794,7 +1791,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B37">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A37, ":"),D$2:D$125)))</f>
@@ -1804,10 +1801,10 @@
         <v>0</v>
       </c>
       <c r="D37" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -1815,20 +1812,20 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B38">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A38, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="E38" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1836,20 +1833,20 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A39, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1857,7 +1854,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B40">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A40, ":"),D$2:D$125)))</f>
@@ -1867,10 +1864,10 @@
         <v>0</v>
       </c>
       <c r="D40" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E40" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -1878,20 +1875,17 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B41">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A41, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
-      <c r="D41" t="s">
-        <v>98</v>
-      </c>
       <c r="E41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G41">
         <v>1</v>
@@ -1899,7 +1893,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B42">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A42, ":"),D$2:D$125)))</f>
@@ -1908,8 +1902,11 @@
       <c r="C42">
         <v>0</v>
       </c>
+      <c r="D42" t="s">
+        <v>99</v>
+      </c>
       <c r="E42" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -1917,20 +1914,20 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B43">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A43, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E43" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1938,7 +1935,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B44">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A44, ":"),D$2:D$125)))</f>
@@ -1948,10 +1945,10 @@
         <v>0</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G44">
         <v>1</v>
@@ -1959,20 +1956,20 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="B45">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A45, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>77</v>
       </c>
       <c r="E45" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -1980,17 +1977,17 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B46">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A46, ":"),D$2:D$125)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>171</v>
       </c>
       <c r="E46" t="s">
         <v>73</v>
@@ -2001,20 +1998,17 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>115</v>
+        <v>5</v>
       </c>
       <c r="B47">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A47, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
-      <c r="D47" t="s">
-        <v>171</v>
-      </c>
       <c r="E47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2022,17 +2016,20 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B48">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A48, ":"),D$2:D$125)))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
+      <c r="D48" t="s">
+        <v>75</v>
+      </c>
       <c r="E48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G48">
         <v>1</v>
@@ -2040,7 +2037,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B49">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A49, ":"),D$2:D$125)))</f>
@@ -2050,10 +2047,10 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G49">
         <v>1</v>
@@ -2061,20 +2058,23 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="B50">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A50, ":"),D$2:D$125)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="E50" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="F50" t="s">
+        <v>158</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2082,23 +2082,23 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>116</v>
+        <v>146</v>
       </c>
       <c r="B51">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A51, ":"),D$2:D$125)))</f>
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>117</v>
+        <v>147</v>
       </c>
       <c r="E51" t="s">
         <v>68</v>
       </c>
       <c r="F51" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="G51">
         <v>1</v>

</xml_diff>

<commit_message>
Added level 2 items. Added new contracts.
</commit_message>
<xml_diff>
--- a/spreadsheets/items.xlsx
+++ b/spreadsheets/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\production-line\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4C3450-E34D-491C-8A41-F1C800AF1940}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BF6D4D-B3A1-4B63-8CAE-659C68CCA50B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37110" windowHeight="14625" xr2:uid="{90F13507-3F9A-4BE5-82EE-4FDD9857C5A2}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Guide to Uses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="185">
   <si>
     <t>Item</t>
   </si>
@@ -349,9 +350,6 @@
     <t>Steel: 2</t>
   </si>
   <si>
-    <t>Iron: 1, Nickel: 1</t>
-  </si>
-  <si>
     <t>Invar: 2</t>
   </si>
   <si>
@@ -538,9 +536,6 @@
     <t>Wafer</t>
   </si>
   <si>
-    <t>Wafer: 4, Silver Plate: 1</t>
-  </si>
-  <si>
     <t>Superconductor</t>
   </si>
   <si>
@@ -556,9 +551,6 @@
     <t>Niobium Ore</t>
   </si>
   <si>
-    <t>Niobium Ore: 8</t>
-  </si>
-  <si>
     <t>Box of Infinite Unsettling Possibilities</t>
   </si>
   <si>
@@ -581,6 +573,21 @@
   </si>
   <si>
     <t>Battery: 1, Engine: 1, Chassis: 1, Frame: 2</t>
+  </si>
+  <si>
+    <t>todo?</t>
+  </si>
+  <si>
+    <t>Wafer: 4, Silver Plate: 1, Window: 1, Frame: 1</t>
+  </si>
+  <si>
+    <t>Iron: 1, Nickel: 1, Coal: 4</t>
+  </si>
+  <si>
+    <t>Niobium Ore: 4, Coal: 8</t>
+  </si>
+  <si>
+    <t>Has Contract</t>
   </si>
 </sst>
 </file>
@@ -662,7 +669,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -673,7 +687,21 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -994,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{642C1486-BA39-4873-8BE1-FD047E7D1A0C}">
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:J81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1005,21 +1033,24 @@
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1028,18 +1059,21 @@
         <v>67</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A2, ":"),D$2:D$125)))</f>
@@ -1049,7 +1083,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>71</v>
@@ -1058,11 +1092,14 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="I2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1079,8 +1116,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1092,7 +1132,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E4" t="s">
         <v>70</v>
@@ -1100,8 +1140,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1113,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" t="s">
         <v>71</v>
@@ -1121,10 +1164,13 @@
       <c r="G5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B6">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A6, ":"),D$2:D$125)))</f>
@@ -1134,21 +1180,24 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
         <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B7">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A7, ":"),D$2:D$125)))</f>
@@ -1158,21 +1207,24 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" t="s">
         <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B8">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A8, ":"),D$2:D$125)))</f>
@@ -1182,19 +1234,22 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E8" t="s">
         <v>68</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
@@ -1212,13 +1267,16 @@
         <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -1235,13 +1293,19 @@
       <c r="E10" t="s">
         <v>68</v>
       </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A11, ":"),D$2:D$125)))</f>
@@ -1251,16 +1315,22 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E11" t="s">
         <v>68</v>
       </c>
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -1277,8 +1347,11 @@
       <c r="G12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1298,8 +1371,11 @@
       <c r="G13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1319,8 +1395,11 @@
       <c r="G14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
@@ -1332,21 +1411,24 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E15" t="s">
         <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B16">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A16, ":"),D$2:D$125)))</f>
@@ -1356,25 +1438,28 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E16" t="s">
         <v>71</v>
       </c>
       <c r="F16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B17">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A17, ":"),D$2:D$125)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1388,8 +1473,11 @@
       <c r="G17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
@@ -1406,11 +1494,17 @@
       <c r="E18" t="s">
         <v>68</v>
       </c>
+      <c r="F18" t="s">
+        <v>157</v>
+      </c>
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1428,13 +1522,16 @@
         <v>68</v>
       </c>
       <c r="F19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -1451,8 +1548,11 @@
       <c r="G20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1472,8 +1572,11 @@
       <c r="G21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
@@ -1493,8 +1596,11 @@
       <c r="G22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
@@ -1511,8 +1617,11 @@
       <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1532,8 +1641,11 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -1551,15 +1663,18 @@
         <v>71</v>
       </c>
       <c r="F25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B26">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A26, ":"),D$2:D$125)))</f>
@@ -1569,19 +1684,22 @@
         <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E26" t="s">
         <v>68</v>
       </c>
       <c r="F26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1598,8 +1716,11 @@
       <c r="G27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>21</v>
       </c>
@@ -1619,8 +1740,11 @@
       <c r="G28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
@@ -1640,8 +1764,11 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1658,8 +1785,11 @@
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
@@ -1679,8 +1809,11 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
@@ -1700,10 +1833,13 @@
       <c r="G32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A33, ":"),D$2:D$125)))</f>
@@ -1713,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>73</v>
@@ -1722,10 +1858,13 @@
       <c r="G33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B34">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$125)))</f>
@@ -1735,19 +1874,22 @@
         <v>1</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>68</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
@@ -1767,8 +1909,11 @@
       <c r="G35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
@@ -1788,8 +1933,11 @@
       <c r="G36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
@@ -1809,8 +1957,11 @@
       <c r="G37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
@@ -1830,8 +1981,11 @@
       <c r="G38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
@@ -1851,8 +2005,11 @@
       <c r="G39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>32</v>
       </c>
@@ -1872,14 +2029,17 @@
       <c r="G40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B41">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A41, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -1890,8 +2050,11 @@
       <c r="G41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
@@ -1911,8 +2074,11 @@
       <c r="G42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
@@ -1932,8 +2098,11 @@
       <c r="G43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
@@ -1953,10 +2122,13 @@
       <c r="G44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A45, ":"),D$2:D$125)))</f>
@@ -1966,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E45" t="s">
         <v>73</v>
@@ -1974,10 +2146,13 @@
       <c r="G45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A46, ":"),D$2:D$125)))</f>
@@ -1987,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E46" t="s">
         <v>73</v>
@@ -1995,8 +2170,11 @@
       <c r="G46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -2013,8 +2191,11 @@
       <c r="G47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -2034,8 +2215,11 @@
       <c r="G48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -2055,10 +2239,13 @@
       <c r="G49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B50">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A50, ":"),D$2:D$125)))</f>
@@ -2068,21 +2255,24 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E50" t="s">
         <v>68</v>
       </c>
       <c r="F50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G50">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A51, ":"),D$2:D$125)))</f>
@@ -2092,21 +2282,24 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E51" t="s">
         <v>68</v>
       </c>
       <c r="F51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G51">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B52">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A52, ":"),D$2:D$125)))</f>
@@ -2121,76 +2314,88 @@
       <c r="G52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B53">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A53, ":"),D$2:D$125)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C53">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="E53" t="s">
-        <v>71</v>
+        <v>68</v>
+      </c>
+      <c r="F53" t="s">
+        <v>157</v>
       </c>
       <c r="G53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>165</v>
+        <v>36</v>
       </c>
       <c r="B54">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A54, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="E54" t="s">
-        <v>68</v>
-      </c>
-      <c r="F54" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="G54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B55">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A55, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B56">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A56, ":"),D$2:D$125)))</f>
@@ -2200,60 +2405,69 @@
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E56" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B57">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A57, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E57" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B58">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A58, ":"),D$2:D$125)))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B59">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A59, ":"),D$2:D$125)))</f>
@@ -2263,57 +2477,66 @@
         <v>0</v>
       </c>
       <c r="D59" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="E59" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B60">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A60, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
-      <c r="D60" t="s">
-        <v>104</v>
-      </c>
       <c r="E60" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B61">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A61, ":"),D$2:D$125)))</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
+      <c r="D61" t="s">
+        <v>79</v>
+      </c>
       <c r="E61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B62">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A62, ":"),D$2:D$125)))</f>
@@ -2323,18 +2546,21 @@
         <v>0</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E62" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>24</v>
+        <v>166</v>
       </c>
       <c r="B63">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A63, ":"),D$2:D$125)))</f>
@@ -2344,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="D63" t="s">
-        <v>87</v>
+        <v>165</v>
       </c>
       <c r="E63" t="s">
         <v>71</v>
@@ -2352,32 +2578,38 @@
       <c r="G63">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B64">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A64, ":"),D$2:D$125)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E64" t="s">
         <v>68</v>
       </c>
       <c r="F64" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="G64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>42</v>
       </c>
@@ -2389,7 +2621,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>105</v>
+        <v>182</v>
       </c>
       <c r="E65" t="s">
         <v>73</v>
@@ -2397,8 +2629,11 @@
       <c r="G65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>43</v>
       </c>
@@ -2418,8 +2653,11 @@
       <c r="G66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>44</v>
       </c>
@@ -2431,7 +2669,7 @@
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E67" t="s">
         <v>71</v>
@@ -2439,8 +2677,11 @@
       <c r="G67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>45</v>
       </c>
@@ -2457,8 +2698,11 @@
       <c r="G68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>46</v>
       </c>
@@ -2478,8 +2722,11 @@
       <c r="G69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>47</v>
       </c>
@@ -2491,7 +2738,7 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E70" t="s">
         <v>71</v>
@@ -2499,10 +2746,13 @@
       <c r="G70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B71">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A71, ":"),D$2:D$125)))</f>
@@ -2514,8 +2764,14 @@
       <c r="E71" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>48</v>
       </c>
@@ -2527,16 +2783,19 @@
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E72" t="s">
         <v>73</v>
       </c>
       <c r="G72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>49</v>
       </c>
@@ -2548,16 +2807,19 @@
         <v>0</v>
       </c>
       <c r="D73" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E73" t="s">
         <v>70</v>
       </c>
       <c r="G73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>50</v>
       </c>
@@ -2569,18 +2831,21 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E74" t="s">
         <v>71</v>
       </c>
       <c r="G74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B75">
         <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A75, ":"),D$2:D$125)))</f>
@@ -2590,19 +2855,22 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E75" t="s">
         <v>73</v>
       </c>
       <c r="F75" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>51</v>
       </c>
@@ -2619,8 +2887,11 @@
       <c r="G76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>52</v>
       </c>
@@ -2632,7 +2903,7 @@
         <v>0</v>
       </c>
       <c r="D77" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E77" t="s">
         <v>70</v>
@@ -2640,8 +2911,11 @@
       <c r="G77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>53</v>
       </c>
@@ -2653,7 +2927,7 @@
         <v>0</v>
       </c>
       <c r="D78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E78" t="s">
         <v>71</v>
@@ -2661,8 +2935,11 @@
       <c r="G78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>54</v>
       </c>
@@ -2674,7 +2951,7 @@
         <v>0</v>
       </c>
       <c r="D79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E79" t="s">
         <v>73</v>
@@ -2682,8 +2959,11 @@
       <c r="G79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>55</v>
       </c>
@@ -2695,7 +2975,7 @@
         <v>0</v>
       </c>
       <c r="D80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E80" t="s">
         <v>70</v>
@@ -2703,8 +2983,11 @@
       <c r="G80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>56</v>
       </c>
@@ -2716,12 +2999,15 @@
         <v>0</v>
       </c>
       <c r="D81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E81" t="s">
         <v>71</v>
       </c>
       <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
         <v>0</v>
       </c>
     </row>
@@ -2743,12 +3029,7 @@
       <formula>(INDIRECT(ADDRESS(ROW(),COLUMN()-4)))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D109">
-    <cfRule type="expression" dxfId="1" priority="8">
-      <formula>ISNUMBER(SEARCH(_xlfn.CONCAT($I$2, ":"),INDIRECT(ADDRESS(ROW(), COLUMN()))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G1048576">
+  <conditionalFormatting sqref="G1:H1048576">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2761,12 +3042,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(D1))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D109">
+    <cfRule type="expression" dxfId="0" priority="9">
+      <formula>ISNUMBER(SEARCH(_xlfn.CONCAT($J$2, ":"),INDIRECT(ADDRESS(ROW(), COLUMN()))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2" xr:uid="{B41CAD5B-3ED5-49EE-9D16-AE4F85D7209A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2" xr:uid="{B41CAD5B-3ED5-49EE-9D16-AE4F85D7209A}">
       <formula1>$A$1:$A$81</formula1>
     </dataValidation>
   </dataValidations>
@@ -2818,15 +3104,15 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2834,7 +3120,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2842,7 +3128,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2850,7 +3136,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2858,7 +3144,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2866,7 +3152,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2874,7 +3160,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2882,7 +3168,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -2890,7 +3176,7 @@
         <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2898,7 +3184,7 @@
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2906,15 +3192,15 @@
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" t="s">
         <v>163</v>
-      </c>
-      <c r="B13" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2922,7 +3208,7 @@
         <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2930,7 +3216,7 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2938,7 +3224,7 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2946,7 +3232,7 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2954,7 +3240,7 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2962,7 +3248,7 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2970,7 +3256,7 @@
         <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more lvl 2 item icons.
</commit_message>
<xml_diff>
--- a/spreadsheets/items.xlsx
+++ b/spreadsheets/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\production-line\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226AEA69-73BF-4DF4-8BAF-3794ED61501E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B06418-E66F-42B3-8A65-EE58D55904C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37110" windowHeight="14625" xr2:uid="{90F13507-3F9A-4BE5-82EE-4FDD9857C5A2}"/>
   </bookViews>
@@ -1196,8 +1196,8 @@
   <dimension ref="A1:M112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2529,7 @@
         <v>68</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2796,7 +2796,7 @@
         <v>68</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2826,7 +2826,7 @@
         <v>157</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2913,7 +2913,7 @@
         <v>156</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -2970,7 +2970,7 @@
         <v>68</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -3000,7 +3000,7 @@
         <v>157</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -3027,7 +3027,7 @@
         <v>68</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -3054,7 +3054,7 @@
         <v>68</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -3249,7 +3249,7 @@
         <v>68</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -3276,7 +3276,7 @@
         <v>68</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -3558,7 +3558,7 @@
         <v>156</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85">
         <v>0</v>

</xml_diff>

<commit_message>
Added remaining level 2 item icons.
</commit_message>
<xml_diff>
--- a/spreadsheets/items.xlsx
+++ b/spreadsheets/items.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\production-line\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B06418-E66F-42B3-8A65-EE58D55904C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2362C38F-7E0D-4201-860C-9A5E0F145B59}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="37110" windowHeight="14625" xr2:uid="{90F13507-3F9A-4BE5-82EE-4FDD9857C5A2}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Guide to Uses" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -614,9 +613,6 @@
     <t>Power Supply</t>
   </si>
   <si>
-    <t>Wire: 3, Frame: 1</t>
-  </si>
-  <si>
     <t>Processor</t>
   </si>
   <si>
@@ -780,6 +776,9 @@
   </si>
   <si>
     <t>Hull: 1, Adv. Engine: 1, Window: 2</t>
+  </si>
+  <si>
+    <t>Chassis: 1, Copper Coil: 2, Wire: 3</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1195,8 @@
   <dimension ref="A1:M112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G86" sqref="G86"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K82" sqref="K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1240,7 @@
         <v>183</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>140</v>
@@ -1253,7 +1252,7 @@
         <v>153</v>
       </c>
       <c r="B2">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A2, ":"),D$2:D$156)))</f>
+        <f t="shared" ref="B2:B33" si="0">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A2, ":"),D$2:D$156)))</f>
         <v>1</v>
       </c>
       <c r="C2" s="6">
@@ -1284,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A3, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C3">
@@ -1308,7 +1307,7 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A4, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C4">
@@ -1335,7 +1334,7 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A5, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C5">
@@ -1362,7 +1361,7 @@
         <v>154</v>
       </c>
       <c r="B6">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A6, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C6">
@@ -1392,7 +1391,7 @@
         <v>143</v>
       </c>
       <c r="B7">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A7, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C7">
@@ -1422,7 +1421,7 @@
         <v>177</v>
       </c>
       <c r="B8">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A8, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C8">
@@ -1452,8 +1451,8 @@
         <v>57</v>
       </c>
       <c r="B9">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A9, ":"),D$2:D$156)))</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1479,7 +1478,7 @@
         <v>58</v>
       </c>
       <c r="B10">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A10, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C10">
@@ -1506,7 +1505,7 @@
         <v>158</v>
       </c>
       <c r="B11">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A11, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="C11">
@@ -1533,7 +1532,7 @@
         <v>4</v>
       </c>
       <c r="B12">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A12, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C12">
@@ -1557,8 +1556,8 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A13, ":"),D$2:D$156)))</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1584,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A14, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14">
@@ -1611,7 +1610,7 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A15, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C15">
@@ -1641,7 +1640,7 @@
         <v>148</v>
       </c>
       <c r="B16">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A16, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="C16">
@@ -1671,8 +1670,8 @@
         <v>59</v>
       </c>
       <c r="B17">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A17, ":"),D$2:D$156)))</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1698,7 +1697,7 @@
         <v>60</v>
       </c>
       <c r="B18">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A18, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C18">
@@ -1728,7 +1727,7 @@
         <v>62</v>
       </c>
       <c r="B19">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A19, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C19">
@@ -1758,7 +1757,7 @@
         <v>6</v>
       </c>
       <c r="B20">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A20, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C20">
@@ -1782,7 +1781,7 @@
         <v>17</v>
       </c>
       <c r="B21">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A21, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C21">
@@ -1809,7 +1808,7 @@
         <v>18</v>
       </c>
       <c r="B22">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A22, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C22">
@@ -1836,7 +1835,7 @@
         <v>7</v>
       </c>
       <c r="B23">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A23, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C23">
@@ -1860,7 +1859,7 @@
         <v>19</v>
       </c>
       <c r="B24">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A24, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C24">
@@ -1887,7 +1886,7 @@
         <v>20</v>
       </c>
       <c r="B25">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A25, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C25">
@@ -1917,7 +1916,7 @@
         <v>173</v>
       </c>
       <c r="B26">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A26, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C26">
@@ -1947,7 +1946,7 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A27, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C27">
@@ -1971,7 +1970,7 @@
         <v>21</v>
       </c>
       <c r="B28">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A28, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C28">
@@ -1998,7 +1997,7 @@
         <v>22</v>
       </c>
       <c r="B29">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A29, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C29">
@@ -2025,7 +2024,7 @@
         <v>8</v>
       </c>
       <c r="B30">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A30, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C30">
@@ -2049,7 +2048,7 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A31, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C31">
@@ -2076,7 +2075,7 @@
         <v>26</v>
       </c>
       <c r="B32">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A32, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C32">
@@ -2103,7 +2102,7 @@
         <v>151</v>
       </c>
       <c r="B33">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A33, ":"),D$2:D$156)))</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C33" s="6">
@@ -2128,17 +2127,17 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="B34">
+        <f t="shared" ref="B34:B65" si="1">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$156)))</f>
+        <v>0</v>
+      </c>
+      <c r="C34" s="6">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>241</v>
-      </c>
-      <c r="B34">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A34, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="6">
-        <v>0</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>242</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>68</v>
@@ -2156,17 +2155,17 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B35">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A35, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C35" s="6">
         <v>0</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>68</v>
@@ -2184,17 +2183,17 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B36">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A36, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C36" s="6">
         <v>0</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>68</v>
@@ -2212,17 +2211,17 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B37">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A37, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C37" s="6">
         <v>0</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>68</v>
@@ -2240,17 +2239,17 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B38">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A38, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>68</v>
@@ -2273,7 +2272,7 @@
         <v>171</v>
       </c>
       <c r="B39">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A39, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C39" s="6">
@@ -2303,7 +2302,7 @@
         <v>27</v>
       </c>
       <c r="B40">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A40, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C40">
@@ -2330,7 +2329,7 @@
         <v>28</v>
       </c>
       <c r="B41">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A41, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C41">
@@ -2357,7 +2356,7 @@
         <v>29</v>
       </c>
       <c r="B42">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A42, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C42">
@@ -2384,7 +2383,7 @@
         <v>30</v>
       </c>
       <c r="B43">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A43, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C43">
@@ -2411,7 +2410,7 @@
         <v>31</v>
       </c>
       <c r="B44">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A44, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C44">
@@ -2438,7 +2437,7 @@
         <v>32</v>
       </c>
       <c r="B45">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A45, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C45">
@@ -2462,17 +2461,17 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
         <v>243</v>
-      </c>
-      <c r="B46">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A46, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46" t="s">
-        <v>244</v>
       </c>
       <c r="E46" t="s">
         <v>68</v>
@@ -2492,7 +2491,7 @@
         <v>3</v>
       </c>
       <c r="B47">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A47, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C47">
@@ -2513,17 +2512,17 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
         <v>196</v>
-      </c>
-      <c r="B48">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A48, ":"),D$2:D$156)))</f>
-        <v>2</v>
-      </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-      <c r="D48" t="s">
-        <v>197</v>
       </c>
       <c r="E48" t="s">
         <v>68</v>
@@ -2543,7 +2542,7 @@
         <v>33</v>
       </c>
       <c r="B49">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A49, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="C49">
@@ -2570,7 +2569,7 @@
         <v>34</v>
       </c>
       <c r="B50">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A50, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C50">
@@ -2597,7 +2596,7 @@
         <v>35</v>
       </c>
       <c r="B51">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A51, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C51">
@@ -2621,17 +2620,17 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
         <v>211</v>
-      </c>
-      <c r="B52">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A52, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
-      <c r="D52" t="s">
-        <v>212</v>
       </c>
       <c r="E52" t="s">
         <v>68</v>
@@ -2651,7 +2650,7 @@
         <v>113</v>
       </c>
       <c r="B53">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A53, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C53">
@@ -2678,7 +2677,7 @@
         <v>114</v>
       </c>
       <c r="B54">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A54, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="C54">
@@ -2705,7 +2704,7 @@
         <v>5</v>
       </c>
       <c r="B55">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A55, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="C55">
@@ -2729,7 +2728,7 @@
         <v>15</v>
       </c>
       <c r="B56">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A56, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C56">
@@ -2756,7 +2755,7 @@
         <v>16</v>
       </c>
       <c r="B57">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A57, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C57">
@@ -2780,17 +2779,17 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58" t="s">
         <v>237</v>
-      </c>
-      <c r="B58">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A58, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>0</v>
-      </c>
-      <c r="D58" t="s">
-        <v>238</v>
       </c>
       <c r="E58" t="s">
         <v>68</v>
@@ -2807,17 +2806,17 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
         <v>233</v>
-      </c>
-      <c r="B59">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A59, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59" t="s">
-        <v>234</v>
       </c>
       <c r="E59" t="s">
         <v>68</v>
@@ -2837,17 +2836,17 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
         <v>209</v>
-      </c>
-      <c r="B60">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A60, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>0</v>
-      </c>
-      <c r="D60" t="s">
-        <v>210</v>
       </c>
       <c r="E60" t="s">
         <v>68</v>
@@ -2867,7 +2866,7 @@
         <v>186</v>
       </c>
       <c r="B61">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A61, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C61">
@@ -2894,17 +2893,17 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
         <v>202</v>
-      </c>
-      <c r="B62">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A62, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>0</v>
-      </c>
-      <c r="D62" t="s">
-        <v>203</v>
       </c>
       <c r="E62" t="s">
         <v>68</v>
@@ -2924,17 +2923,17 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63" t="s">
         <v>235</v>
-      </c>
-      <c r="B63">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A63, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63" t="s">
-        <v>236</v>
       </c>
       <c r="E63" t="s">
         <v>68</v>
@@ -2943,7 +2942,7 @@
         <v>157</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -2954,17 +2953,17 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B64">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A64, ":"),D$2:D$156)))</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E64" t="s">
         <v>68</v>
@@ -2981,17 +2980,17 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
         <v>222</v>
-      </c>
-      <c r="B65">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A65, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65" t="s">
-        <v>223</v>
       </c>
       <c r="E65" t="s">
         <v>68</v>
@@ -3011,17 +3010,17 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B66">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A66, ":"),D$2:D$156)))</f>
+        <f t="shared" ref="B66:B97" si="2">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A66, ":"),D$2:D$156)))</f>
         <v>1</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E66" t="s">
         <v>68</v>
@@ -3038,17 +3037,17 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B67">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A67, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E67" t="s">
         <v>68</v>
@@ -3068,7 +3067,7 @@
         <v>115</v>
       </c>
       <c r="B68">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A68, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C68">
@@ -3098,7 +3097,7 @@
         <v>144</v>
       </c>
       <c r="B69">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A69, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C69">
@@ -3125,17 +3124,17 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70" t="s">
         <v>205</v>
-      </c>
-      <c r="B70">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A70, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C70">
-        <v>0</v>
-      </c>
-      <c r="D70" t="s">
-        <v>206</v>
       </c>
       <c r="E70" t="s">
         <v>68</v>
@@ -3152,17 +3151,17 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
         <v>207</v>
-      </c>
-      <c r="B71">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A71, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C71">
-        <v>0</v>
-      </c>
-      <c r="D71" t="s">
-        <v>208</v>
       </c>
       <c r="E71" t="s">
         <v>68</v>
@@ -3182,20 +3181,20 @@
         <v>192</v>
       </c>
       <c r="B72">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A72, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="E72" t="s">
         <v>68</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -3206,23 +3205,23 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
         <v>194</v>
       </c>
-      <c r="B73">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A73, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C73">
-        <v>0</v>
-      </c>
-      <c r="D73" t="s">
-        <v>195</v>
-      </c>
       <c r="E73" t="s">
         <v>68</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -3233,17 +3232,17 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74" t="s">
         <v>198</v>
-      </c>
-      <c r="B74">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A74, ":"),D$2:D$156)))</f>
-        <v>2</v>
-      </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74" t="s">
-        <v>199</v>
       </c>
       <c r="E74" t="s">
         <v>68</v>
@@ -3260,17 +3259,17 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75" t="s">
         <v>200</v>
-      </c>
-      <c r="B75">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A75, ":"),D$2:D$156)))</f>
-        <v>1</v>
-      </c>
-      <c r="C75">
-        <v>0</v>
-      </c>
-      <c r="D75" t="s">
-        <v>201</v>
       </c>
       <c r="E75" t="s">
         <v>68</v>
@@ -3290,7 +3289,7 @@
         <v>161</v>
       </c>
       <c r="B76">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A76, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C76">
@@ -3314,7 +3313,7 @@
         <v>163</v>
       </c>
       <c r="B77">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A77, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C77">
@@ -3344,7 +3343,7 @@
         <v>36</v>
       </c>
       <c r="B78">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A78, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C78">
@@ -3371,7 +3370,7 @@
         <v>37</v>
       </c>
       <c r="B79">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A79, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C79">
@@ -3384,7 +3383,7 @@
         <v>70</v>
       </c>
       <c r="F79" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G79">
         <v>1</v>
@@ -3401,7 +3400,7 @@
         <v>38</v>
       </c>
       <c r="B80">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A80, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C80">
@@ -3414,7 +3413,7 @@
         <v>71</v>
       </c>
       <c r="F80" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -3431,7 +3430,7 @@
         <v>39</v>
       </c>
       <c r="B81">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A81, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="C81">
@@ -3458,7 +3457,7 @@
         <v>40</v>
       </c>
       <c r="B82">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A82, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C82">
@@ -3485,7 +3484,7 @@
         <v>41</v>
       </c>
       <c r="B83">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A83, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="C83">
@@ -3509,23 +3508,23 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
         <v>213</v>
       </c>
-      <c r="B84">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A84, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
+        <v>68</v>
+      </c>
+      <c r="F84" t="s">
         <v>214</v>
-      </c>
-      <c r="E84" t="s">
-        <v>68</v>
-      </c>
-      <c r="F84" t="s">
-        <v>215</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -3539,17 +3538,17 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85" t="s">
         <v>227</v>
-      </c>
-      <c r="B85">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A85, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
-      </c>
-      <c r="D85" t="s">
-        <v>228</v>
       </c>
       <c r="E85" t="s">
         <v>68</v>
@@ -3569,17 +3568,17 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
+      </c>
+      <c r="D86" t="s">
         <v>231</v>
-      </c>
-      <c r="B86">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A86, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>232</v>
       </c>
       <c r="E86" t="s">
         <v>68</v>
@@ -3588,7 +3587,7 @@
         <v>157</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -3602,7 +3601,7 @@
         <v>10</v>
       </c>
       <c r="B87">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A87, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C87">
@@ -3626,7 +3625,7 @@
         <v>23</v>
       </c>
       <c r="B88">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A88, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C88">
@@ -3653,7 +3652,7 @@
         <v>24</v>
       </c>
       <c r="B89">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A89, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="C89">
@@ -3680,7 +3679,7 @@
         <v>187</v>
       </c>
       <c r="B90">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A90, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C90">
@@ -3710,7 +3709,7 @@
         <v>184</v>
       </c>
       <c r="B91">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A91, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C91">
@@ -3740,7 +3739,7 @@
         <v>165</v>
       </c>
       <c r="B92">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A92, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C92">
@@ -3764,17 +3763,17 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B93">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93" t="s">
         <v>229</v>
-      </c>
-      <c r="B93">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A93, ":"),D$2:D$156)))</f>
-        <v>0</v>
-      </c>
-      <c r="C93">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
-        <v>230</v>
       </c>
       <c r="E93" t="s">
         <v>68</v>
@@ -3783,7 +3782,7 @@
         <v>157</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -3797,7 +3796,7 @@
         <v>117</v>
       </c>
       <c r="B94">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A94, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C94">
@@ -3827,7 +3826,7 @@
         <v>190</v>
       </c>
       <c r="B95">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A95, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="C95">
@@ -3857,7 +3856,7 @@
         <v>42</v>
       </c>
       <c r="B96">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A96, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="C96">
@@ -3884,7 +3883,7 @@
         <v>43</v>
       </c>
       <c r="B97">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A97, ":"),D$2:D$156)))</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="C97">
@@ -3911,7 +3910,7 @@
         <v>44</v>
       </c>
       <c r="B98">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A98, ":"),D$2:D$156)))</f>
+        <f t="shared" ref="B98:B129" si="3">SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A98, ":"),D$2:D$156)))</f>
         <v>0</v>
       </c>
       <c r="C98">
@@ -3938,7 +3937,7 @@
         <v>45</v>
       </c>
       <c r="B99">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A99, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="C99">
@@ -3962,7 +3961,7 @@
         <v>46</v>
       </c>
       <c r="B100">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A100, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C100">
@@ -3989,7 +3988,7 @@
         <v>47</v>
       </c>
       <c r="B101">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A101, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C101">
@@ -4016,7 +4015,7 @@
         <v>170</v>
       </c>
       <c r="B102">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A102, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C102">
@@ -4040,7 +4039,7 @@
         <v>48</v>
       </c>
       <c r="B103">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A103, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="C103">
@@ -4067,7 +4066,7 @@
         <v>49</v>
       </c>
       <c r="B104">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A104, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="C104">
@@ -4094,7 +4093,7 @@
         <v>50</v>
       </c>
       <c r="B105">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A105, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C105">
@@ -4121,7 +4120,7 @@
         <v>166</v>
       </c>
       <c r="B106">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A106, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C106">
@@ -4151,7 +4150,7 @@
         <v>51</v>
       </c>
       <c r="B107">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A107, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="C107">
@@ -4175,7 +4174,7 @@
         <v>52</v>
       </c>
       <c r="B108">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A108, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C108">
@@ -4202,7 +4201,7 @@
         <v>53</v>
       </c>
       <c r="B109">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A109, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C109">
@@ -4229,7 +4228,7 @@
         <v>54</v>
       </c>
       <c r="B110">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A110, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="C110">
@@ -4256,7 +4255,7 @@
         <v>55</v>
       </c>
       <c r="B111">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A111, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C111">
@@ -4283,7 +4282,7 @@
         <v>56</v>
       </c>
       <c r="B112">
-        <f>SUMPRODUCT( -- ISNUMBER(SEARCH(_xlfn.CONCAT(A112, ":"),D$2:D$156)))</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="C112">

</xml_diff>